<commit_message>
0.0.6: Enable force specifying telegramPackage.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTask.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C34B8D-008B-9B4A-9A0C-82D35D31757A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7079AA0F-1678-0947-A629-6593B3CAEA50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -416,6 +416,35 @@
     </rPh>
     <rPh sb="25" eb="27">
       <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>telegrampackage</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>電文の基底クラスが配備されているパッケージを指定します。指定がない場合はvalueobjectから探します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">キテイ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">ハイビ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>シテイシマス。</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">シテイガ </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t xml:space="preserve">サガシマス。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1366,7 +1395,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1410,7 +1439,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1438,7 +1467,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1643,7 +1672,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A28" si="0">A15+1</f>
+        <f t="shared" ref="A16:A29" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -1935,12 +1964,21 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="27"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="A29" s="27">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D29" s="29"/>
       <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="F29" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
       <c r="I29" s="31"/>

</xml_diff>

<commit_message>
0.0.10: Generate application class skeletons, if genSkeleton and other options are specified.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTask.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7079AA0F-1678-0947-A629-6593B3CAEA50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C8984-DA9E-9C42-A31C-65E93392B3CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -445,6 +445,98 @@
     </rPh>
     <rPh sb="49" eb="50">
       <t xml:space="preserve">サガシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>impledir</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>実装ファイルの配置ディレクトリを指定します。controllerから呼び出されるmanagementクラスのスケルトンはここに生成されます。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ジッソウファイル </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ハイチ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t xml:space="preserve">ヨビダサレル </t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>genSkeleton</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>controllerから呼び出されるmanagementクラスのスケルトンを生成します。既にファイルが存在する場合は上書きしません。</t>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">ヨビダサレル </t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t xml:space="preserve">スデニ </t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t xml:space="preserve">ソンザイスル </t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t xml:space="preserve">ウワガキ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>skeletonDelegateClass</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>実装クラスが処理を委譲するクラスのCanonical名です。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">ショリヲ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">イジョウスル </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>skeletonDelegateInterface</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>実装クラスが処理を委譲するクラスが実装するIntefaceのCanonical名です。</t>
+    <rPh sb="5" eb="6">
+      <t>ガ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ショリヲ </t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t xml:space="preserve">イジョウスル </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">ジッソウスル </t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t xml:space="preserve">メイ </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1395,7 +1487,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1439,7 +1531,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1467,7 +1559,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1672,7 +1764,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A29" si="0">A15+1</f>
+        <f t="shared" ref="A16:A33" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -1985,48 +2077,86 @@
       <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="27">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
+      <c r="F30" s="31" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="31"/>
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="27">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>63</v>
+      </c>
       <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
+      <c r="E31" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
       <c r="I31" s="31"/>
       <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="27">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
+      <c r="F32" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="G32" s="31"/>
       <c r="H32" s="31"/>
       <c r="I32" s="31"/>
       <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="27"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
+      <c r="A33" s="27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="29"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
+      <c r="F33" s="31" t="s">
+        <v>74</v>
+      </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
       <c r="I33" s="31"/>

</xml_diff>

<commit_message>
0.0.14: lineSeparator option is implemented.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTask.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C8984-DA9E-9C42-A31C-65E93392B3CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB7998-A419-C345-8D8C-AA0B488B46D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -538,6 +538,18 @@
     <rPh sb="39" eb="40">
       <t xml:space="preserve">メイ </t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>lineSeparator</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>行末記号をしていします。LF=0x0a, CR=0x0d, CFLF=0x0d0x0a とします。LFがデフォルトです。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>LF</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1487,7 +1499,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1531,7 +1543,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1559,7 +1571,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2163,12 +2175,22 @@
       <c r="J33" s="32"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="27"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
+      <c r="A34" s="27">
+        <v>21</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
+      <c r="E34" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>76</v>
+      </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
       <c r="I34" s="31"/>

</xml_diff>

<commit_message>
3.1.2: Implement appendApplicationPackage option. * append "application" package to Management Class. * default is true.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTask.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/vscode/blanco/blancoRestGeneratorKt/meta/program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E425AA05-1376-A24F-AE5D-6AA27E6304A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD9B237-2DC0-8E45-8260-C9E99774A4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -804,6 +804,20 @@
     </rPh>
     <rPh sb="106" eb="108">
       <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>appendApplicationPackage</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Management クラスの package として、Controller クラスの package に application を追加したものを想定し、importします。</t>
+    <rPh sb="67" eb="69">
+      <t xml:space="preserve">ツイカ </t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t xml:space="preserve">ソウテイシマス </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1412,6 +1426,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1434,15 +1457,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1835,7 +1849,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1879,7 +1893,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1906,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:J42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1952,10 +1966,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="66"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="6" t="s">
         <v>50</v>
       </c>
@@ -1965,10 +1979,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="66"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="10" t="s">
         <v>51</v>
       </c>
@@ -1978,10 +1992,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="66"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="6" t="s">
         <v>52</v>
       </c>
@@ -1993,10 +2007,10 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="66"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
@@ -2030,40 +2044,40 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="67"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16">
@@ -2112,7 +2126,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="22">
-        <f t="shared" ref="A16:A42" si="0">A15+1</f>
+        <f t="shared" ref="A16:A43" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -2282,12 +2296,12 @@
       <c r="E23" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
       <c r="J23" s="27"/>
     </row>
     <row r="24" spans="1:10">
@@ -2692,21 +2706,32 @@
       <c r="E42" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="72"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="63"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
+      <c r="A43" s="22">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>63</v>
+      </c>
       <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="26"/>
+      <c r="E43" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>98</v>
+      </c>
       <c r="G43" s="26"/>
       <c r="H43" s="26"/>
       <c r="I43" s="26"/>
@@ -2750,18 +2775,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F42:J42"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:J13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="F42:J42"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:J13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">

</xml_diff>

<commit_message>
Add no bracket option for array query parameters.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtTask.xlsx
+++ b/meta/program/BlancoRestGeneratorKtTask.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1AD46B-F81A-614B-AF7F-33218D0BEE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35E7A9FB-C534-7541-A26B-DEED8AC94248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3980" yWindow="1640" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anttask" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -856,10 +857,7 @@
   <si>
     <t>「必須」が指定されていないパラメータに@Nullableアノテーションを強制します</t>
     <rPh sb="0" eb="2">
-      <t xml:space="preserve">デンブｎ </t>
-    </rPh>
-    <rPh sb="56" eb="58">
-      <t xml:space="preserve">フヨシマス。 </t>
+      <t xml:space="preserve">デンブｎ フヨシマス。 </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1468,16 +1466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -1507,6 +1495,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1900,7 +1898,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1944,7 +1942,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1971,7 +1969,7 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -2017,10 +2015,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="63"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="6" t="s">
         <v>50</v>
       </c>
@@ -2030,10 +2028,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="63"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="10" t="s">
         <v>51</v>
       </c>
@@ -2043,10 +2041,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="63"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="6" t="s">
         <v>52</v>
       </c>
@@ -2058,10 +2056,10 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="63"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
@@ -2095,40 +2093,40 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="77" t="s">
+      <c r="F12" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16">
@@ -2347,12 +2345,12 @@
       <c r="E23" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="73" t="s">
+      <c r="F23" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
       <c r="J23" s="27"/>
     </row>
     <row r="24" spans="1:10">
@@ -2757,13 +2755,13 @@
       <c r="E42" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="72"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="68"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="22">
@@ -2780,13 +2778,13 @@
       <c r="E43" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="65" t="s">
+      <c r="F43" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="67"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="22">
@@ -2803,13 +2801,13 @@
       <c r="E44" s="25" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="68" t="s">
+      <c r="F44" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="69"/>
-      <c r="J44" s="69"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="22">
@@ -2895,6 +2893,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="F43:J43"/>
     <mergeCell ref="F44:J44"/>
     <mergeCell ref="F42:J42"/>
@@ -2902,13 +2907,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:J13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">

</xml_diff>